<commit_message>
newest changes to bigram model
</commit_message>
<xml_diff>
--- a/neural-network/bigram-pattern-frequencies/for-mlp/bigram-pattern-frequencies-test.xlsx
+++ b/neural-network/bigram-pattern-frequencies/for-mlp/bigram-pattern-frequencies-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\Downloads\projects\3-zadanie-4-tyzden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a66692c83fa18ac/Desktop/temp/relationships-between-organizational-patterns/relationships-between-organizational-patterns/bigram-pattern-frequencies/for-mlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AA13C1-EE56-492A-B7C9-1C182EB77115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{87AA13C1-EE56-492A-B7C9-1C182EB77115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FE0195E-5C7E-4BA6-B096-29DE35185EFA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Apprenticeship</t>
   </si>
@@ -83,18 +83,56 @@
   </si>
   <si>
     <t>0.89</t>
+  </si>
+  <si>
+    <t>FewRoles</t>
+  </si>
+  <si>
+    <t>GenericsAndSpecifics</t>
+  </si>
+  <si>
+    <t>SubclassPerTeam</t>
+  </si>
+  <si>
+    <t>HierarchyOfFactories</t>
+  </si>
+  <si>
+    <t>LooseInterfaces</t>
+  </si>
+  <si>
+    <t>ParserBuilder</t>
+  </si>
+  <si>
+    <t>ArchitectControlsProduct</t>
+  </si>
+  <si>
+    <t>DeployAlongTheGrain</t>
+  </si>
+  <si>
+    <t>DeveloperControlsProcess</t>
+  </si>
+  <si>
+    <t>ArchitectureTeam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,19 +193,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,6 +863,457 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M9" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D10" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L10" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M10" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.29</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2.67</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M13" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L15" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M15" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K16" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L16" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M17" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J18" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K18" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L18" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3.04</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="J19" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="K19" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="L19" s="5">
+        <v>1.01</v>
+      </c>
+      <c r="M19" s="5">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>